<commit_message>
assistente cadastro - prestador de serviço
</commit_message>
<xml_diff>
--- a/Documentação/Requisitos-Jobby-Jobs.xlsx
+++ b/Documentação/Requisitos-Jobby-Jobs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buna_\Desktop\3 SEMESTRE\PI 3\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\Desktop\20201-3adsa-grupo9\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB36385-3F60-4C66-978B-24AE8ED54DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="105">
   <si>
     <t>Proposto</t>
   </si>
@@ -462,11 +463,14 @@
   <si>
     <t>O usuário deve ter opção para fazer upload</t>
   </si>
+  <si>
+    <t>Disponibilizar dark mode para usuarios</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23">
     <font>
       <sz val="10"/>
@@ -1094,6 +1098,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,9 +1172,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1669,27 +1673,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="D7:U32" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D7:U32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U32" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D7:U32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Descrição do Requisito" dataDxfId="17"/>
-    <tableColumn id="2" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
-    <tableColumn id="3" name="Prioridade" dataDxfId="15"/>
-    <tableColumn id="4" name="Versão do Requisito" dataDxfId="14"/>
-    <tableColumn id="7" name="Tipo Requisito " dataDxfId="13"/>
-    <tableColumn id="8" name="Complexidade" dataDxfId="12"/>
-    <tableColumn id="9" name="Solicitante" dataDxfId="11"/>
-    <tableColumn id="10" name="Responsável" dataDxfId="10"/>
-    <tableColumn id="11" name="Validador" dataDxfId="9"/>
-    <tableColumn id="12" name="Critérios de Aceitação" dataDxfId="8"/>
-    <tableColumn id="13" name="Dependência Internas entre Requisitos  (rastreabilidade)" dataDxfId="7"/>
-    <tableColumn id="14" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
-    <tableColumn id="15" name="Data da Criação" dataDxfId="5"/>
-    <tableColumn id="16" name="Data Última Alteração" dataDxfId="4"/>
-    <tableColumn id="17" name="Responsável pela última alteração" dataDxfId="3"/>
-    <tableColumn id="18" name="Motivo Última Alteração" dataDxfId="2"/>
-    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="1"/>
-    <tableColumn id="20" name="Situação do Requisito" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prioridade" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Versão do Requisito" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo Requisito " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complexidade" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Solicitante" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Responsável" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Validador" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Critérios de Aceitação" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Dependência Internas entre Requisitos  (rastreabilidade)" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Data da Criação" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Data Última Alteração" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Responsável pela última alteração" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Motivo Última Alteração" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Documentação de Apoio" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Situação do Requisito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1771,6 +1775,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1806,6 +1827,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1981,7 +2019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2000,12 +2038,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="4" spans="2:5" ht="27" customHeight="1">
       <c r="B4" s="6" t="s">
@@ -2116,14 +2154,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:W37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2174,22 +2212,22 @@
       <c r="U1" s="12"/>
     </row>
     <row r="2" spans="2:23" ht="16.5" customHeight="1" thickBot="1">
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="67" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="67"/>
+      <c r="P2" s="68"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="16"/>
       <c r="T2" s="17" t="s">
@@ -2198,40 +2236,40 @@
       <c r="U2" s="12"/>
     </row>
     <row r="3" spans="2:23" ht="14.25" customHeight="1" thickBot="1">
-      <c r="E3" s="64"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="69"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
       <c r="Q3" s="7"/>
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:23" ht="12.75" customHeight="1" thickBot="1">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="70" t="s">
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="70"/>
+      <c r="P4" s="71"/>
       <c r="Q4" s="12"/>
       <c r="S4" s="18"/>
       <c r="T4" s="19"/>
@@ -2240,18 +2278,18 @@
     <row r="5" spans="2:23">
       <c r="B5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="72"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="73"/>
       <c r="Q5" s="20"/>
       <c r="S5" s="18"/>
       <c r="T5" s="19"/>
@@ -2259,18 +2297,18 @@
     </row>
     <row r="6" spans="2:23" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
       <c r="C6" s="22"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="74"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="75"/>
       <c r="Q6" s="23"/>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
@@ -3261,10 +3299,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:23" s="39" customFormat="1" ht="15.75">
-      <c r="B24" s="40"/>
+    <row r="24" spans="2:23" s="39" customFormat="1" ht="27">
+      <c r="B24" s="40">
+        <v>10</v>
+      </c>
       <c r="C24" s="41"/>
-      <c r="D24" s="34"/>
+      <c r="D24" s="34" t="s">
+        <v>104</v>
+      </c>
       <c r="E24" s="35"/>
       <c r="F24" s="36" t="s">
         <v>52</v>
@@ -3696,7 +3738,7 @@
       </c>
     </row>
     <row r="37" spans="9:9">
-      <c r="I37" s="75"/>
+      <c r="I37" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3709,21 +3751,21 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U32" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I32" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H32" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="T27" r:id="rId1"/>
-    <hyperlink ref="T28" r:id="rId2"/>
-    <hyperlink ref="T29" r:id="rId3"/>
-    <hyperlink ref="T30" r:id="rId4"/>
+    <hyperlink ref="T27" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="T28" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="T29" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="T30" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId5"/>

</xml_diff>

<commit_message>
ppt - sprint 02
</commit_message>
<xml_diff>
--- a/Documentação/Requisitos-Jobby-Jobs.xlsx
+++ b/Documentação/Requisitos-Jobby-Jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\Desktop\20201-3adsa-grupo9\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB36385-3F60-4C66-978B-24AE8ED54DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300FB4C0-1EAC-4D7E-A9A9-71080B94E5BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="103">
   <si>
     <t>Proposto</t>
   </si>
@@ -293,12 +293,6 @@
     <t>Home deve conter as informações do produto</t>
   </si>
   <si>
-    <t>Home deve conter as informações da equipe</t>
-  </si>
-  <si>
-    <t>Usuário conhecer a equipe do produto</t>
-  </si>
-  <si>
     <t>Avaliação das funcionalidades e se está de acordo com o solicitante</t>
   </si>
   <si>
@@ -404,42 +398,21 @@
     <t>Página do contratante</t>
   </si>
   <si>
-    <t>Página do contratante deve conter filtros por avaliação de "funcionários"</t>
-  </si>
-  <si>
-    <t>Escolha de funcionário através de filtro</t>
-  </si>
-  <si>
-    <t>Página do contratante deve conter conter comentários de avaliação de "funcionários"</t>
-  </si>
-  <si>
-    <t>Escolha de funcionário através de avaliação</t>
-  </si>
-  <si>
     <t>Verificar se a visualização dos comentários estão corretos</t>
   </si>
   <si>
     <t>Verificar se a aplicação de filtros funciona corretamente</t>
   </si>
   <si>
-    <t xml:space="preserve">Página do empregado informal </t>
-  </si>
-  <si>
     <t xml:space="preserve">Verificar se os dados estão corretos </t>
   </si>
   <si>
-    <t xml:space="preserve">Página do empregado informal deve conter campos para descrição de sua função, objetivo, preço do serviço, foto do empregado, breve descrição de seriços prestados e campo para recomendação de contratantes </t>
-  </si>
-  <si>
     <t xml:space="preserve">Usuário conhecer o serviço que está contratando </t>
   </si>
   <si>
     <t>Verificar se os dados do usuário e entrada de dados estão corretos</t>
   </si>
   <si>
-    <t xml:space="preserve">Página de cadastro deve conter campos para selecionar se é um usuário contrante ou usuário empregado </t>
-  </si>
-  <si>
     <t>Diferentes tipos de cadastro para usuários</t>
   </si>
   <si>
@@ -465,6 +438,27 @@
   </si>
   <si>
     <t>Disponibilizar dark mode para usuarios</t>
+  </si>
+  <si>
+    <t>Página do contratante deve conter filtros por avaliação de "babás"</t>
+  </si>
+  <si>
+    <t>Escolha de babás através de filtro</t>
+  </si>
+  <si>
+    <t>Página do contratante deve conter conter comentários de avaliação de "babás"</t>
+  </si>
+  <si>
+    <t>Escolha de babás através de avaliação</t>
+  </si>
+  <si>
+    <t>Página da babá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Página da babá deve conter campos para descrição de sua função, objetivo, preço do serviço, foto do empregado, breve descrição de seriços prestados e campo para recomendação de contratantes </t>
+  </si>
+  <si>
+    <t>Página de cadastro deve conter campos para selecionar se é um usuário contrante ou babá</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1667,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U32" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D7:U32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U31" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D7:U31" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
@@ -2067,7 +2061,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="48">
         <v>44067</v>
@@ -2078,10 +2072,10 @@
         <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="48">
         <v>44099</v>
@@ -2155,13 +2149,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:W37"/>
+  <dimension ref="B1:W36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2255,7 +2249,7 @@
     </row>
     <row r="4" spans="2:23" ht="12.75" customHeight="1" thickBot="1">
       <c r="E4" s="53" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="54"/>
       <c r="G4" s="54"/>
@@ -2404,35 +2398,35 @@
         <v>44</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L8" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N8" s="35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O8" s="34"/>
       <c r="P8" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q8" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R8" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S8" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T8" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U8" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:23" s="39" customFormat="1" ht="54">
@@ -2462,50 +2456,50 @@
         <v>44</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L9" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N9" s="35" t="s">
         <v>10</v>
       </c>
       <c r="O9" s="34"/>
       <c r="P9" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q9" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R9" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S9" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T9" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U9" s="36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="2:23" s="39" customFormat="1" ht="54">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41" t="s">
-        <v>35</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" s="39" customFormat="1" ht="67.5">
+      <c r="B10" s="40">
+        <v>2</v>
+      </c>
+      <c r="C10" s="41"/>
       <c r="D10" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>10</v>
@@ -2514,56 +2508,56 @@
         <v>33</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L10" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N10" s="35" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="O10" s="34"/>
       <c r="P10" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q10" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S10" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T10" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="U10" s="44" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="U10" s="36" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="2:23" s="39" customFormat="1" ht="67.5">
-      <c r="B11" s="40">
-        <v>2</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="34" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>50</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>52</v>
       </c>
       <c r="G11" s="36" t="s">
         <v>10</v>
@@ -2571,57 +2565,57 @@
       <c r="H11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="36" t="s">
-        <v>42</v>
+      <c r="I11" s="42" t="s">
+        <v>62</v>
       </c>
       <c r="J11" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K11" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="L11" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M11" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="35" t="s">
-        <v>79</v>
       </c>
       <c r="O11" s="34"/>
       <c r="P11" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q11" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R11" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S11" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T11" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U11" s="36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="2:23" s="39" customFormat="1" ht="67.5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" s="39" customFormat="1" ht="54">
       <c r="B12" s="40"/>
       <c r="C12" s="41" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" s="36" t="s">
         <v>10</v>
@@ -2630,56 +2624,56 @@
         <v>33</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="J12" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K12" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L12" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M12" s="36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N12" s="35" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="O12" s="34"/>
       <c r="P12" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q12" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R12" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S12" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T12" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U12" s="36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="2:23" s="39" customFormat="1" ht="54">
-      <c r="B13" s="40"/>
-      <c r="C13" s="41" t="s">
-        <v>82</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" s="39" customFormat="1" ht="67.5">
+      <c r="B13" s="40">
+        <v>4</v>
+      </c>
+      <c r="C13" s="41"/>
       <c r="D13" s="38" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G13" s="36" t="s">
         <v>10</v>
@@ -2688,56 +2682,56 @@
         <v>33</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J13" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K13" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M13" s="36" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="O13" s="34"/>
       <c r="P13" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q13" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R13" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S13" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T13" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U13" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:23" s="39" customFormat="1" ht="67.5">
+    <row r="14" spans="2:23" s="39" customFormat="1" ht="40.5">
       <c r="B14" s="40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="41"/>
-      <c r="D14" s="38" t="s">
-        <v>57</v>
+      <c r="D14" s="34" t="s">
+        <v>81</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G14" s="36" t="s">
         <v>10</v>
@@ -2745,122 +2739,122 @@
       <c r="H14" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="42" t="s">
-        <v>43</v>
+      <c r="I14" s="36" t="s">
+        <v>42</v>
       </c>
       <c r="J14" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K14" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="L14" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M14" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="35" t="s">
-        <v>26</v>
       </c>
       <c r="O14" s="34"/>
       <c r="P14" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q14" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R14" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S14" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T14" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U14" s="36" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:23" s="39" customFormat="1" ht="40.5">
-      <c r="B15" s="40">
-        <v>5</v>
-      </c>
-      <c r="C15" s="41"/>
+      <c r="W14" s="46"/>
+    </row>
+    <row r="15" spans="2:23" s="39" customFormat="1" ht="89.25" customHeight="1">
+      <c r="B15" s="40"/>
+      <c r="C15" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="D15" s="34" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J15" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="36" t="s">
-        <v>78</v>
+      <c r="K15" s="44" t="s">
+        <v>76</v>
       </c>
       <c r="L15" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="N15" s="35" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="O15" s="34"/>
       <c r="P15" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q15" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R15" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S15" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T15" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U15" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="W15" s="46"/>
-    </row>
-    <row r="16" spans="2:23" s="39" customFormat="1" ht="89.25" customHeight="1">
+    </row>
+    <row r="16" spans="2:23" s="39" customFormat="1" ht="54">
       <c r="B16" s="40"/>
       <c r="C16" s="41" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G16" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I16" s="36" t="s">
         <v>43</v>
@@ -2869,50 +2863,50 @@
         <v>44</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L16" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M16" s="36" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N16" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O16" s="34"/>
       <c r="P16" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q16" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R16" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S16" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T16" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U16" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:23" s="39" customFormat="1" ht="54">
-      <c r="B17" s="40"/>
-      <c r="C17" s="41" t="s">
-        <v>65</v>
-      </c>
+    <row r="17" spans="2:23" s="39" customFormat="1" ht="67.5">
+      <c r="B17" s="40">
+        <v>6</v>
+      </c>
+      <c r="C17" s="41"/>
       <c r="D17" s="34" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G17" s="36" t="s">
         <v>10</v>
@@ -2921,62 +2915,62 @@
         <v>33</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="L17" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="L17" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M17" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="N17" s="35" t="s">
-        <v>61</v>
       </c>
       <c r="O17" s="34"/>
       <c r="P17" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q17" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R17" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S17" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="T17" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="T17" s="38" t="s">
+        <v>52</v>
       </c>
       <c r="U17" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:23" s="39" customFormat="1" ht="67.5">
-      <c r="B18" s="40">
-        <v>6</v>
-      </c>
-      <c r="C18" s="41"/>
+    <row r="18" spans="2:23" s="39" customFormat="1" ht="81">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="D18" s="34" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" s="36" t="s">
         <v>42</v>
@@ -2985,50 +2979,51 @@
         <v>44</v>
       </c>
       <c r="K18" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L18" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M18" s="36" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="N18" s="35" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="O18" s="34"/>
       <c r="P18" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q18" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R18" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S18" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T18" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U18" s="36" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:23" s="39" customFormat="1" ht="81">
-      <c r="B19" s="40"/>
-      <c r="C19" s="41" t="s">
-        <v>69</v>
-      </c>
+      <c r="W18" s="46"/>
+    </row>
+    <row r="19" spans="2:23" s="39" customFormat="1" ht="54">
+      <c r="B19" s="40">
+        <v>7</v>
+      </c>
+      <c r="C19" s="41"/>
       <c r="D19" s="34" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G19" s="36" t="s">
         <v>10</v>
@@ -3043,51 +3038,50 @@
         <v>44</v>
       </c>
       <c r="K19" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="L19" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="N19" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="L19" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M19" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="N19" s="35" t="s">
-        <v>34</v>
       </c>
       <c r="O19" s="34"/>
       <c r="P19" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q19" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R19" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S19" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T19" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U19" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="W19" s="46"/>
-    </row>
-    <row r="20" spans="2:23" s="39" customFormat="1" ht="54">
+    </row>
+    <row r="20" spans="2:23" s="39" customFormat="1" ht="40.5">
       <c r="B20" s="40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="34" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G20" s="36" t="s">
         <v>10</v>
@@ -3102,50 +3096,50 @@
         <v>44</v>
       </c>
       <c r="K20" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="L20" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M20" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>80</v>
       </c>
       <c r="O20" s="34"/>
       <c r="P20" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q20" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R20" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S20" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T20" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U20" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:23" s="39" customFormat="1" ht="40.5">
+    <row r="21" spans="2:23" s="39" customFormat="1" ht="94.5">
       <c r="B21" s="40">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="34" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G21" s="36" t="s">
         <v>10</v>
@@ -3157,53 +3151,49 @@
         <v>42</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="K21" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L21" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M21" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N21" s="35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O21" s="34"/>
       <c r="P21" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q21" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R21" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S21" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T21" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U21" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:23" s="39" customFormat="1" ht="94.5">
-      <c r="B22" s="40">
-        <v>9</v>
-      </c>
+    <row r="22" spans="2:23" s="39" customFormat="1" ht="15.75">
+      <c r="B22" s="40"/>
       <c r="C22" s="41"/>
-      <c r="D22" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>74</v>
-      </c>
+      <c r="D22" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="35"/>
       <c r="F22" s="36" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="G22" s="36" t="s">
         <v>10</v>
@@ -3212,52 +3202,50 @@
         <v>32</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="K22" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L22" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M22" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="N22" s="35" t="s">
-        <v>79</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="M22" s="36"/>
+      <c r="N22" s="35"/>
       <c r="O22" s="34"/>
       <c r="P22" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q22" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R22" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S22" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T22" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U22" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:23" s="39" customFormat="1" ht="15.75">
-      <c r="B23" s="40"/>
+    <row r="23" spans="2:23" s="39" customFormat="1" ht="27">
+      <c r="B23" s="40">
+        <v>10</v>
+      </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="49" t="s">
-        <v>103</v>
+      <c r="D23" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="E23" s="35"/>
       <c r="F23" s="36" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G23" s="36" t="s">
         <v>10</v>
@@ -3266,50 +3254,46 @@
         <v>32</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J23" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K23" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L23" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M23" s="36"/>
       <c r="N23" s="35"/>
       <c r="O23" s="34"/>
       <c r="P23" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q23" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R23" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S23" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T23" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U23" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:23" s="39" customFormat="1" ht="27">
-      <c r="B24" s="40">
-        <v>10</v>
-      </c>
+    <row r="24" spans="2:23" s="39" customFormat="1" ht="15.75">
+      <c r="B24" s="40"/>
       <c r="C24" s="41"/>
-      <c r="D24" s="34" t="s">
-        <v>104</v>
-      </c>
+      <c r="D24" s="34"/>
       <c r="E24" s="35"/>
       <c r="F24" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G24" s="36" t="s">
         <v>10</v>
@@ -3318,34 +3302,34 @@
         <v>32</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J24" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K24" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L24" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M24" s="36"/>
       <c r="N24" s="35"/>
       <c r="O24" s="34"/>
       <c r="P24" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q24" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R24" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S24" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T24" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U24" s="36" t="s">
         <v>0</v>
@@ -3357,13 +3341,13 @@
       <c r="D25" s="34"/>
       <c r="E25" s="35"/>
       <c r="F25" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G25" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I25" s="36" t="s">
         <v>43</v>
@@ -3372,28 +3356,28 @@
         <v>44</v>
       </c>
       <c r="K25" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L25" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M25" s="36"/>
       <c r="N25" s="35"/>
       <c r="O25" s="34"/>
       <c r="P25" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q25" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R25" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S25" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T25" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U25" s="36" t="s">
         <v>0</v>
@@ -3402,58 +3386,58 @@
     <row r="26" spans="2:23" s="39" customFormat="1" ht="15.75">
       <c r="B26" s="40"/>
       <c r="C26" s="41"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="35"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G26" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H26" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J26" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K26" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L26" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M26" s="36"/>
+        <v>76</v>
+      </c>
+      <c r="M26" s="47"/>
       <c r="N26" s="35"/>
       <c r="O26" s="34"/>
       <c r="P26" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q26" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R26" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S26" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="T26" s="38" t="s">
-        <v>54</v>
+        <v>77</v>
+      </c>
+      <c r="T26" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="U26" s="36" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:23" s="39" customFormat="1" ht="15.75">
       <c r="B27" s="40"/>
       <c r="C27" s="41"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
       <c r="F27" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G27" s="36" t="s">
         <v>10</v>
@@ -3468,31 +3452,31 @@
         <v>44</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L27" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M27" s="47"/>
+        <v>76</v>
+      </c>
+      <c r="M27" s="36"/>
       <c r="N27" s="35"/>
       <c r="O27" s="34"/>
       <c r="P27" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q27" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R27" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S27" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T27" s="45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U27" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:23" s="39" customFormat="1" ht="15.75">
@@ -3501,7 +3485,7 @@
       <c r="D28" s="34"/>
       <c r="E28" s="35"/>
       <c r="F28" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G28" s="36" t="s">
         <v>10</v>
@@ -3516,31 +3500,31 @@
         <v>44</v>
       </c>
       <c r="K28" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L28" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M28" s="36"/>
       <c r="N28" s="35"/>
       <c r="O28" s="34"/>
       <c r="P28" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q28" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R28" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S28" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T28" s="45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U28" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="2:23" s="39" customFormat="1" ht="15.75">
@@ -3549,10 +3533,10 @@
       <c r="D29" s="34"/>
       <c r="E29" s="35"/>
       <c r="F29" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G29" s="36" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H29" s="36" t="s">
         <v>32</v>
@@ -3564,31 +3548,31 @@
         <v>44</v>
       </c>
       <c r="K29" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L29" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M29" s="36"/>
       <c r="N29" s="35"/>
       <c r="O29" s="34"/>
       <c r="P29" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q29" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R29" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S29" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T29" s="45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U29" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="2:23" s="39" customFormat="1" ht="15.75">
@@ -3597,46 +3581,48 @@
       <c r="D30" s="34"/>
       <c r="E30" s="35"/>
       <c r="F30" s="36" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G30" s="36" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="H30" s="36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J30" s="36" t="s">
         <v>44</v>
       </c>
       <c r="K30" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L30" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M30" s="36"/>
-      <c r="N30" s="35"/>
+      <c r="N30" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="O30" s="34"/>
       <c r="P30" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q30" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R30" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S30" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="T30" s="45" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="T30" s="38" t="s">
+        <v>52</v>
       </c>
       <c r="U30" s="36" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:23" s="39" customFormat="1" ht="15.75">
@@ -3645,7 +3631,7 @@
       <c r="D31" s="34"/>
       <c r="E31" s="35"/>
       <c r="F31" s="36" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G31" s="36" t="s">
         <v>10</v>
@@ -3660,85 +3646,35 @@
         <v>44</v>
       </c>
       <c r="K31" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L31" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M31" s="36"/>
-      <c r="N31" s="35" t="s">
-        <v>101</v>
-      </c>
+      <c r="N31" s="35"/>
       <c r="O31" s="34"/>
       <c r="P31" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q31" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R31" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S31" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T31" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U31" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:23" s="39" customFormat="1" ht="15.75">
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="J32" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="K32" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="L32" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M32" s="36"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q32" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="R32" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="S32" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="T32" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="U32" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9">
-      <c r="I37" s="51"/>
+    <row r="36" spans="9:9">
+      <c r="I36" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3751,21 +3687,21 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U32" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U31" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I32" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I31" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H32" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H31" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="T27" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="T28" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="T29" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="T30" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="T26" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="T27" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="T28" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="T29" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId5"/>

</xml_diff>